<commit_message>
update examples to avoid deprecated functions
</commit_message>
<xml_diff>
--- a/db_files/extractions_mislabelling_sheet.xlsx
+++ b/db_files/extractions_mislabelling_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdsel\Documents\Google Drive\TAMUCC-CORE\PIRE\database_albatross_recollections\db_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C5F729-5100-4E42-BBB1-798E9F78F2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DCCA27-A4EF-4D58-A7B1-CFA753D440DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{0B1C575A-E7F5-402B-B6AE-B21BDB3269A2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{0B1C575A-E7F5-402B-B6AE-B21BDB3269A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="101">
-  <si>
-    <t>Extraction_ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="155">
   <si>
     <t>Corrected_Extraction_ID</t>
   </si>
@@ -53,9 +50,6 @@
     <t>Pba-CCab_097_Ex1</t>
   </si>
   <si>
-    <t>Individual_ID</t>
-  </si>
-  <si>
     <t>Corrected_Individual_ID</t>
   </si>
   <si>
@@ -65,9 +59,6 @@
     <t>Pba-CCab_066</t>
   </si>
   <si>
-    <t>Sequence_ID</t>
-  </si>
-  <si>
     <t>Corrected_Sequence_ID</t>
   </si>
   <si>
@@ -77,9 +68,6 @@
     <t>Pba-CCab_097-Ex1-8B-lcwgs-1-1</t>
   </si>
   <si>
-    <t>Lot_ID</t>
-  </si>
-  <si>
     <t>Corrected_Lot_ID</t>
   </si>
   <si>
@@ -89,15 +77,9 @@
     <t>Duplicate Individuals labelled as Pba-CCab_066. Changed number to 097. 8.18.25 JDS/CEB</t>
   </si>
   <si>
-    <t>Extraction_Plate_ID</t>
-  </si>
-  <si>
     <t>Mix-C_011</t>
   </si>
   <si>
-    <t>Extraction_Plate_Well_Address</t>
-  </si>
-  <si>
     <t>2F</t>
   </si>
   <si>
@@ -339,6 +321,186 @@
   </si>
   <si>
     <t>Extraction for individual 002 labelled as 001 causing subsequent extractions to be mislabelled too</t>
+  </si>
+  <si>
+    <t>Original_Lot_ID</t>
+  </si>
+  <si>
+    <t>Original_Individual_ID</t>
+  </si>
+  <si>
+    <t>Original_Extraction_ID</t>
+  </si>
+  <si>
+    <t>Original_Extraction_Plate_ID</t>
+  </si>
+  <si>
+    <t>Original_Extraction_Plate_Well_Address</t>
+  </si>
+  <si>
+    <t>Original_Sequence_ID</t>
+  </si>
+  <si>
+    <t>Gma-CPas_001</t>
+  </si>
+  <si>
+    <t>Gma-CPas_001-Ex1</t>
+  </si>
+  <si>
+    <t>Gma-CPas_002</t>
+  </si>
+  <si>
+    <t>Gma-CPas_002-Ex1</t>
+  </si>
+  <si>
+    <t>Gma-CPas_003</t>
+  </si>
+  <si>
+    <t>Gma-CPas_003-Ex1</t>
+  </si>
+  <si>
+    <t>Gma-CPas_004</t>
+  </si>
+  <si>
+    <t>Gma-CPas_004-Ex1</t>
+  </si>
+  <si>
+    <t>Gma-CPas_005</t>
+  </si>
+  <si>
+    <t>Gma-CPas_005-Ex1</t>
+  </si>
+  <si>
+    <t>Gma-CPas_006</t>
+  </si>
+  <si>
+    <t>Gma-CPas_006-Ex1</t>
+  </si>
+  <si>
+    <t>Gma-CPas_007</t>
+  </si>
+  <si>
+    <t>Gma-CPas_007-Ex1</t>
+  </si>
+  <si>
+    <t>Gma-CPas_008</t>
+  </si>
+  <si>
+    <t>Gma-CPas_008-Ex1</t>
+  </si>
+  <si>
+    <t>Gma-CRag_001</t>
+  </si>
+  <si>
+    <t>Gma-CRag_002</t>
+  </si>
+  <si>
+    <t>Gma-CRag_003</t>
+  </si>
+  <si>
+    <t>Gma-CRag_004</t>
+  </si>
+  <si>
+    <t>Gma-CRag_005</t>
+  </si>
+  <si>
+    <t>Gma-CRag_006</t>
+  </si>
+  <si>
+    <t>Gma-CRag_007</t>
+  </si>
+  <si>
+    <t>Gma-CRag_008</t>
+  </si>
+  <si>
+    <t>Gma-CRag_001-Ex1</t>
+  </si>
+  <si>
+    <t>Gma-CRag_002-Ex1</t>
+  </si>
+  <si>
+    <t>Gma-CRag_003-Ex1</t>
+  </si>
+  <si>
+    <t>Gma-CRag_004-Ex1</t>
+  </si>
+  <si>
+    <t>Gma-CRag_005-Ex1</t>
+  </si>
+  <si>
+    <t>Gma-CRag_006-Ex1</t>
+  </si>
+  <si>
+    <t>Gma-CRag_007-Ex1</t>
+  </si>
+  <si>
+    <t>Gma-CRag_008-Ex1</t>
+  </si>
+  <si>
+    <t>Mix-C_005</t>
+  </si>
+  <si>
+    <t>Mix-C_005, Mix-C_007</t>
+  </si>
+  <si>
+    <t>1C</t>
+  </si>
+  <si>
+    <t>2C</t>
+  </si>
+  <si>
+    <t>3C</t>
+  </si>
+  <si>
+    <t>4C</t>
+  </si>
+  <si>
+    <t>5C</t>
+  </si>
+  <si>
+    <t>6C</t>
+  </si>
+  <si>
+    <t>7C</t>
+  </si>
+  <si>
+    <t>8C</t>
+  </si>
+  <si>
+    <t>Cam-2019-013_019</t>
+  </si>
+  <si>
+    <t>Cam-2019-017_029</t>
+  </si>
+  <si>
+    <t>Location labelled as Rag not Pas</t>
+  </si>
+  <si>
+    <t>Incorrect location ID</t>
+  </si>
+  <si>
+    <t>misID_013</t>
+  </si>
+  <si>
+    <t>misID_014</t>
+  </si>
+  <si>
+    <t>misID_015</t>
+  </si>
+  <si>
+    <t>misID_016</t>
+  </si>
+  <si>
+    <t>misID_017</t>
+  </si>
+  <si>
+    <t>misID_018</t>
+  </si>
+  <si>
+    <t>misID_019</t>
+  </si>
+  <si>
+    <t>misID_020</t>
   </si>
 </sst>
 </file>
@@ -750,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E8183B-0B23-476D-B9F4-8C3AC8DE7AF0}">
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,663 +936,1069 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>95</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>5</v>
+        <v>96</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="P1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>2</v>
       </c>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" t="s">
-        <v>4</v>
-      </c>
       <c r="L2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="N2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="O2" s="4">
         <v>45887</v>
       </c>
       <c r="P2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="Q2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C3" s="5">
         <v>97445</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="I3" s="5">
         <v>97445</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="L3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="M3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="N3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="O3" s="4">
         <v>45888</v>
       </c>
       <c r="P3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Q3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C4" s="5">
         <v>97445</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="I4" s="5">
         <v>97445</v>
       </c>
       <c r="J4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="K4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="M4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="N4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="O4" s="4">
         <v>45888</v>
       </c>
       <c r="P4" t="s">
-        <v>99</v>
+        <v>93</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C5" s="5">
         <v>97445</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I5" s="5">
         <v>97445</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="K5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="L5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="M5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="N5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="O5" s="4">
         <v>45888</v>
       </c>
       <c r="P5" t="s">
-        <v>99</v>
+        <v>93</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C6" s="5">
         <v>97445</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="H6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="I6" s="5">
         <v>97445</v>
       </c>
       <c r="J6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="K6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="L6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="M6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="N6" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="O6" s="4">
         <v>45888</v>
       </c>
       <c r="P6" t="s">
-        <v>99</v>
+        <v>93</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C7" s="5">
         <v>97536</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="I7" s="5">
         <v>97536</v>
       </c>
       <c r="J7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="K7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="L7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="M7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="N7" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="O7" s="4">
         <v>45888</v>
       </c>
       <c r="P7" t="s">
-        <v>99</v>
+        <v>93</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" t="s">
         <v>92</v>
-      </c>
-      <c r="B8" t="s">
-        <v>98</v>
       </c>
       <c r="C8" s="5">
         <v>97536</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" t="s">
         <v>76</v>
       </c>
-      <c r="G8" t="s">
-        <v>82</v>
-      </c>
       <c r="H8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="I8" s="5">
         <v>97536</v>
       </c>
       <c r="J8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="L8" t="s">
+        <v>70</v>
+      </c>
+      <c r="M8" t="s">
         <v>76</v>
       </c>
-      <c r="M8" t="s">
-        <v>82</v>
-      </c>
       <c r="N8" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="O8" s="4">
         <v>45888</v>
       </c>
       <c r="P8" t="s">
-        <v>99</v>
+        <v>93</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C9" s="5">
         <v>97536</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F9" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G9" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H9" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="I9" s="5">
         <v>97536</v>
       </c>
       <c r="J9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="K9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="L9" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="M9" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="N9" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="O9" s="4">
         <v>45888</v>
       </c>
       <c r="P9" t="s">
-        <v>99</v>
+        <v>93</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C10" s="5">
         <v>97521</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F10" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G10" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="I10" s="5">
         <v>97521</v>
       </c>
       <c r="J10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="K10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="L10" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="M10" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="N10" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="O10" s="4">
         <v>45888</v>
       </c>
       <c r="P10" t="s">
-        <v>99</v>
+        <v>93</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C11" s="5">
         <v>97521</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F11" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G11" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H11" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I11" s="5">
         <v>97521</v>
       </c>
       <c r="J11" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="K11" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="L11" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="M11" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="N11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="O11" s="4">
         <v>45888</v>
       </c>
       <c r="P11" t="s">
-        <v>99</v>
+        <v>93</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B12" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C12" s="5">
         <v>97521</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F12" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G12" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H12" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="I12" s="5">
         <v>97521</v>
       </c>
       <c r="J12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="K12" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="L12" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="M12" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="N12" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="O12" s="4">
         <v>45888</v>
       </c>
       <c r="P12" t="s">
-        <v>99</v>
+        <v>93</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B13" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C13" s="6">
         <v>97617</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F13" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G13" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="H13" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="I13" s="6">
         <v>97617</v>
       </c>
       <c r="J13" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="K13" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="L13" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="M13" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="N13" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="O13" s="4">
         <v>45888</v>
       </c>
       <c r="P13" t="s">
-        <v>99</v>
+        <v>93</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" t="s">
+        <v>117</v>
+      </c>
+      <c r="E14" t="s">
+        <v>125</v>
+      </c>
+      <c r="F14" t="s">
+        <v>133</v>
+      </c>
+      <c r="G14" t="s">
+        <v>135</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="J14" t="s">
+        <v>101</v>
+      </c>
+      <c r="K14" t="s">
+        <v>102</v>
+      </c>
+      <c r="L14" t="s">
+        <v>133</v>
+      </c>
+      <c r="M14" t="s">
+        <v>135</v>
+      </c>
+      <c r="O14" s="4">
+        <v>45887</v>
+      </c>
+      <c r="P14" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D15" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" t="s">
+        <v>126</v>
+      </c>
+      <c r="F15" t="s">
+        <v>134</v>
+      </c>
+      <c r="G15" t="s">
+        <v>136</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="J15" t="s">
+        <v>103</v>
+      </c>
+      <c r="K15" t="s">
+        <v>104</v>
+      </c>
+      <c r="L15" t="s">
+        <v>134</v>
+      </c>
+      <c r="M15" t="s">
+        <v>136</v>
+      </c>
+      <c r="O15" s="4">
+        <v>45887</v>
+      </c>
+      <c r="P15" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>149</v>
+      </c>
+      <c r="B16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D16" t="s">
+        <v>119</v>
+      </c>
+      <c r="E16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F16" t="s">
+        <v>133</v>
+      </c>
+      <c r="G16" t="s">
+        <v>137</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="J16" t="s">
+        <v>105</v>
+      </c>
+      <c r="K16" t="s">
+        <v>106</v>
+      </c>
+      <c r="L16" t="s">
+        <v>133</v>
+      </c>
+      <c r="M16" t="s">
+        <v>137</v>
+      </c>
+      <c r="O16" s="4">
+        <v>45887</v>
+      </c>
+      <c r="P16" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D17" t="s">
+        <v>120</v>
+      </c>
+      <c r="E17" t="s">
+        <v>128</v>
+      </c>
+      <c r="F17" t="s">
+        <v>133</v>
+      </c>
+      <c r="G17" t="s">
+        <v>138</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="J17" t="s">
+        <v>107</v>
+      </c>
+      <c r="K17" t="s">
+        <v>108</v>
+      </c>
+      <c r="L17" t="s">
+        <v>133</v>
+      </c>
+      <c r="M17" t="s">
+        <v>138</v>
+      </c>
+      <c r="O17" s="4">
+        <v>45887</v>
+      </c>
+      <c r="P17" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B18" t="s">
+        <v>146</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" t="s">
+        <v>121</v>
+      </c>
+      <c r="E18" t="s">
+        <v>129</v>
+      </c>
+      <c r="F18" t="s">
+        <v>133</v>
+      </c>
+      <c r="G18" t="s">
+        <v>139</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="J18" t="s">
+        <v>109</v>
+      </c>
+      <c r="K18" t="s">
+        <v>110</v>
+      </c>
+      <c r="L18" t="s">
+        <v>133</v>
+      </c>
+      <c r="M18" t="s">
+        <v>139</v>
+      </c>
+      <c r="O18" s="4">
+        <v>45887</v>
+      </c>
+      <c r="P18" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B19" t="s">
+        <v>146</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D19" t="s">
+        <v>122</v>
+      </c>
+      <c r="E19" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19" t="s">
+        <v>133</v>
+      </c>
+      <c r="G19" t="s">
+        <v>140</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="J19" t="s">
+        <v>111</v>
+      </c>
+      <c r="K19" t="s">
+        <v>112</v>
+      </c>
+      <c r="L19" t="s">
+        <v>133</v>
+      </c>
+      <c r="M19" t="s">
+        <v>140</v>
+      </c>
+      <c r="O19" s="4">
+        <v>45887</v>
+      </c>
+      <c r="P19" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>153</v>
+      </c>
+      <c r="B20" t="s">
+        <v>146</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D20" t="s">
+        <v>123</v>
+      </c>
+      <c r="E20" t="s">
+        <v>131</v>
+      </c>
+      <c r="F20" t="s">
+        <v>133</v>
+      </c>
+      <c r="G20" t="s">
+        <v>141</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="J20" t="s">
+        <v>113</v>
+      </c>
+      <c r="K20" t="s">
+        <v>114</v>
+      </c>
+      <c r="L20" t="s">
+        <v>133</v>
+      </c>
+      <c r="M20" t="s">
+        <v>141</v>
+      </c>
+      <c r="O20" s="4">
+        <v>45887</v>
+      </c>
+      <c r="P20" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>154</v>
+      </c>
+      <c r="B21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D21" t="s">
+        <v>124</v>
+      </c>
+      <c r="E21" t="s">
+        <v>132</v>
+      </c>
+      <c r="F21" t="s">
+        <v>133</v>
+      </c>
+      <c r="G21" t="s">
+        <v>142</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="J21" t="s">
+        <v>115</v>
+      </c>
+      <c r="K21" t="s">
+        <v>116</v>
+      </c>
+      <c r="L21" t="s">
+        <v>133</v>
+      </c>
+      <c r="M21" t="s">
+        <v>142</v>
+      </c>
+      <c r="O21" s="4">
+        <v>45887</v>
+      </c>
+      <c r="P21" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>